<commit_message>
I MADE EVERYTHING RED
</commit_message>
<xml_diff>
--- a/Tentative Schedule with SE Minor.xlsx
+++ b/Tentative Schedule with SE Minor.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="80" windowWidth="22980" windowHeight="9520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$O$40</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -252,12 +257,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,17 +283,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,407 +606,410 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="5"/>
+    <col min="6" max="6" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="5"/>
+    <col min="10" max="10" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="J2" s="5" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="K3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="4" spans="1:12">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D4" s="5">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="H4" s="5">
+        <v>4</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="L4" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="6" spans="1:12">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6" s="5">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="H6" s="5">
+        <v>4</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="L6" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="H7" s="5">
+        <v>4</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
+      <c r="L7" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="C10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <f>SUM(D4:D9)</f>
         <v>16</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="5">
         <f>SUM(H4:H9)</f>
         <v>16</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="5">
         <f>SUM(L4:L9)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:12">
+      <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="F12" s="5" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="F12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="J12" s="5" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="J12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="B13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="G13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="K13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="14" spans="1:12">
+      <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H14">
-        <v>4</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="H14" s="5">
+        <v>4</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="15" spans="1:12">
+      <c r="B15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="D15" s="5">
+        <v>4</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H15">
-        <v>4</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="H15" s="5">
+        <v>4</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="L15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="L15" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="D16" s="5">
+        <v>4</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H16">
-        <v>4</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="H16" s="5">
+        <v>4</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="L16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="L16" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="D17" s="5">
+        <v>4</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H17">
-        <v>4</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="H17" s="5">
+        <v>4</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="L17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="L17" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C20" s="2" t="s">
+      <c r="D18" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="C20" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="5">
         <f>SUM(D14:D19)</f>
         <v>17</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="5">
         <f>SUM(H14:H19)</f>
         <v>16</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="5">
         <f>SUM(L14:L19)</f>
         <v>14</v>
       </c>
@@ -1001,7 +1024,12 @@
     <mergeCell ref="J12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="46" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="46" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1013,9 +1041,9 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -1023,31 +1051,31 @@
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="J1" s="5" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1076,7 +1104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1105,7 +1133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -1134,7 +1162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -1163,7 +1191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1197,27 +1225,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="F11" s="5" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="F11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="J11" s="5" t="s">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="J11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1246,7 +1274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="B13" t="s">
         <v>29</v>
       </c>
@@ -1275,7 +1303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="B14" t="s">
         <v>31</v>
       </c>
@@ -1304,7 +1332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="B15" t="s">
         <v>33</v>
       </c>
@@ -1333,7 +1361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="J16" s="3" t="s">
         <v>35</v>
       </c>
@@ -1344,10 +1372,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12">
       <c r="B17" s="3"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12">
       <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1370,7 +1398,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12">
       <c r="B22" t="s">
         <v>48</v>
       </c>
@@ -1381,7 +1409,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12">
       <c r="C23" t="s">
         <v>65</v>
       </c>
@@ -1389,7 +1417,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12">
       <c r="C24" t="s">
         <v>66</v>
       </c>
@@ -1407,6 +1435,11 @@
     <mergeCell ref="J11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1416,8 +1449,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>